<commit_message>
[Senendra] Refactor: Refactoring errors in sending email
</commit_message>
<xml_diff>
--- a/Contacts From Database.xlsx
+++ b/Contacts From Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehil\Desktop\AddressBookSystem-BluePrism\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Senendra Deshlahre\Desktop\BluePrism-AddressBookSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F174AD-CA8C-4DDB-8227-D47276B85A1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D739914-F790-4616-91E5-42466EC89EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3130" yWindow="1630" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="1545" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,84 +25,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>zip</t>
-  </si>
-  <si>
-    <t>phone_number</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Shreyas</t>
-  </si>
-  <si>
-    <t>Iyer</t>
-  </si>
-  <si>
-    <t>1000 Michigan Ave.</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t>Shreyas@gmail.com</t>
-  </si>
-  <si>
-    <t>Shikhar</t>
-  </si>
-  <si>
-    <t>Dhawan</t>
-  </si>
-  <si>
-    <t>1000 Harbor Ave.</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>Shikhar@gmail.com</t>
-  </si>
-  <si>
-    <t>Johny</t>
-  </si>
-  <si>
-    <t>Bairstow</t>
-  </si>
-  <si>
-    <t>200 Baker Street</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>Johny@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shikhar                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhawan                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 Harbor Ave.                                                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seattle                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WA                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shikhar@gmail.com                                                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johny                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bairstow                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 Baker Street                                                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">English                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johny@gmail.com                                                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shreyas                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iyer                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 Michigan Ave.                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicago                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shreyas@gmail.com                                                                                   </t>
   </si>
 </sst>
 </file>
@@ -420,13 +420,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,21 +457,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>60605</v>
@@ -475,24 +480,24 @@
         <v>3889233120</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>98116</v>
@@ -501,24 +506,24 @@
         <v>8332443923</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>57575</v>
@@ -527,7 +532,59 @@
         <v>5645645666</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>98116</v>
+      </c>
+      <c r="G5">
+        <v>8332443923</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>57575</v>
+      </c>
+      <c r="G6">
+        <v>5645645666</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>